<commit_message>
updated pipeline with pipeline scripts sourced from 00pipeline_setup.R" git status ls
</commit_message>
<xml_diff>
--- a/SFBR_mapping_files/Mapping_Files.xlsx
+++ b/SFBR_mapping_files/Mapping_Files.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Priv\Broad River Pathogen Study\Metagenomics\SFBR_60_metagenomics_2013_WY\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10995" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Manure_Study" sheetId="1" r:id="rId1"/>
     <sheet name="SFBR60_RE" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SFBR60_RE!$A$1:$H$147</definedName>
     <definedName name="manure_mapping" localSheetId="0">Manure_Study!$A$1:$G$131</definedName>
     <definedName name="manure_mapping" localSheetId="1">SFBR60_RE!$A$1:$G$131</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="451">
   <si>
     <t>#SampleID</t>
   </si>
@@ -1386,6 +1385,21 @@
   </si>
   <si>
     <t>SFBR60_IS09</t>
+  </si>
+  <si>
+    <t>rise</t>
+  </si>
+  <si>
+    <t>peak</t>
+  </si>
+  <si>
+    <t>fall</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>Flow_Type</t>
   </si>
 </sst>
 </file>
@@ -1393,9 +1407,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="hh:mm"/>
+    <numFmt numFmtId="164" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1406,6 +1420,22 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1428,22 +1458,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="10">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -1511,7 +1556,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1546,7 +1591,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1723,7 +1768,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1737,12 +1782,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="7" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1765,17 +1810,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1798,7 +1843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1821,7 +1866,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1844,7 +1889,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1867,7 +1912,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1890,7 +1935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1913,7 +1958,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1936,7 +1981,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1959,7 +2004,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1982,7 +2027,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2005,7 +2050,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -2028,7 +2073,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2051,7 +2096,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -2074,7 +2119,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -2097,7 +2142,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -2120,7 +2165,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -2143,7 +2188,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -2166,7 +2211,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -2189,7 +2234,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -2212,7 +2257,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -2235,7 +2280,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -2258,7 +2303,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>89</v>
       </c>
@@ -2281,7 +2326,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -2304,7 +2349,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -2327,7 +2372,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -2350,7 +2395,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -2373,7 +2418,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>107</v>
       </c>
@@ -2396,7 +2441,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -2419,7 +2464,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -2442,7 +2487,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>118</v>
       </c>
@@ -2465,7 +2510,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>121</v>
       </c>
@@ -2488,7 +2533,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -2511,7 +2556,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>127</v>
       </c>
@@ -2534,7 +2579,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>130</v>
       </c>
@@ -2557,7 +2602,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>133</v>
       </c>
@@ -2580,7 +2625,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>136</v>
       </c>
@@ -2603,7 +2648,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>139</v>
       </c>
@@ -2626,7 +2671,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>142</v>
       </c>
@@ -2649,7 +2694,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>145</v>
       </c>
@@ -2672,7 +2717,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>148</v>
       </c>
@@ -2695,7 +2740,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>151</v>
       </c>
@@ -2718,7 +2763,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>154</v>
       </c>
@@ -2741,7 +2786,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>157</v>
       </c>
@@ -2764,7 +2809,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>160</v>
       </c>
@@ -2787,7 +2832,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>163</v>
       </c>
@@ -2810,7 +2855,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>166</v>
       </c>
@@ -2833,7 +2878,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>169</v>
       </c>
@@ -2856,7 +2901,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>172</v>
       </c>
@@ -2879,7 +2924,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>175</v>
       </c>
@@ -2902,7 +2947,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>178</v>
       </c>
@@ -2925,7 +2970,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>181</v>
       </c>
@@ -2948,7 +2993,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>184</v>
       </c>
@@ -2971,7 +3016,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>187</v>
       </c>
@@ -2994,7 +3039,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>190</v>
       </c>
@@ -3017,7 +3062,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>193</v>
       </c>
@@ -3040,7 +3085,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>196</v>
       </c>
@@ -3063,7 +3108,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>199</v>
       </c>
@@ -3086,7 +3131,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>202</v>
       </c>
@@ -3109,7 +3154,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>205</v>
       </c>
@@ -3132,7 +3177,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>208</v>
       </c>
@@ -3155,7 +3200,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>211</v>
       </c>
@@ -3178,7 +3223,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>214</v>
       </c>
@@ -3201,7 +3246,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>217</v>
       </c>
@@ -3224,7 +3269,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>220</v>
       </c>
@@ -3247,7 +3292,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>223</v>
       </c>
@@ -3270,7 +3315,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>226</v>
       </c>
@@ -3293,7 +3338,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>229</v>
       </c>
@@ -3316,7 +3361,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>232</v>
       </c>
@@ -3339,7 +3384,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>235</v>
       </c>
@@ -3362,7 +3407,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>238</v>
       </c>
@@ -3385,7 +3430,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>241</v>
       </c>
@@ -3408,7 +3453,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>244</v>
       </c>
@@ -3431,7 +3476,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>247</v>
       </c>
@@ -3454,7 +3499,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>250</v>
       </c>
@@ -3477,7 +3522,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>253</v>
       </c>
@@ -3500,7 +3545,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>256</v>
       </c>
@@ -3523,7 +3568,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>259</v>
       </c>
@@ -3546,7 +3591,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>262</v>
       </c>
@@ -3569,7 +3614,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>265</v>
       </c>
@@ -3592,7 +3637,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>268</v>
       </c>
@@ -3615,7 +3660,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>271</v>
       </c>
@@ -3638,7 +3683,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>274</v>
       </c>
@@ -3661,7 +3706,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>277</v>
       </c>
@@ -3684,7 +3729,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>280</v>
       </c>
@@ -3707,7 +3752,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>283</v>
       </c>
@@ -3730,7 +3775,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>286</v>
       </c>
@@ -3753,7 +3798,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>289</v>
       </c>
@@ -3776,7 +3821,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>292</v>
       </c>
@@ -3799,7 +3844,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>295</v>
       </c>
@@ -3822,7 +3867,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>298</v>
       </c>
@@ -3845,7 +3890,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>301</v>
       </c>
@@ -3868,7 +3913,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>304</v>
       </c>
@@ -3891,7 +3936,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>307</v>
       </c>
@@ -3914,7 +3959,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
         <v>310</v>
       </c>
@@ -3937,7 +3982,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7">
       <c r="A98" t="s">
         <v>313</v>
       </c>
@@ -3960,7 +4005,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
         <v>316</v>
       </c>
@@ -3983,7 +4028,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" t="s">
         <v>319</v>
       </c>
@@ -4006,7 +4051,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
         <v>322</v>
       </c>
@@ -4029,7 +4074,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" t="s">
         <v>325</v>
       </c>
@@ -4052,7 +4097,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" t="s">
         <v>328</v>
       </c>
@@ -4075,7 +4120,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" t="s">
         <v>331</v>
       </c>
@@ -4098,7 +4143,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7">
       <c r="A105" t="s">
         <v>334</v>
       </c>
@@ -4121,7 +4166,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7">
       <c r="A106" t="s">
         <v>337</v>
       </c>
@@ -4144,7 +4189,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7">
       <c r="A107" t="s">
         <v>340</v>
       </c>
@@ -4167,7 +4212,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7">
       <c r="A108" t="s">
         <v>343</v>
       </c>
@@ -4190,7 +4235,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7">
       <c r="A109" t="s">
         <v>346</v>
       </c>
@@ -4213,7 +4258,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7">
       <c r="A110" t="s">
         <v>349</v>
       </c>
@@ -4236,7 +4281,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7">
       <c r="A111" t="s">
         <v>352</v>
       </c>
@@ -4259,7 +4304,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7">
       <c r="A112" t="s">
         <v>355</v>
       </c>
@@ -4282,7 +4327,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7">
       <c r="A113" t="s">
         <v>358</v>
       </c>
@@ -4305,7 +4350,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7">
       <c r="A114" t="s">
         <v>361</v>
       </c>
@@ -4328,7 +4373,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7">
       <c r="A115" t="s">
         <v>364</v>
       </c>
@@ -4351,7 +4396,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7">
       <c r="A116" t="s">
         <v>367</v>
       </c>
@@ -4374,7 +4419,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7">
       <c r="A117" t="s">
         <v>370</v>
       </c>
@@ -4397,7 +4442,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7">
       <c r="A118" t="s">
         <v>373</v>
       </c>
@@ -4420,7 +4465,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7">
       <c r="A119" t="s">
         <v>376</v>
       </c>
@@ -4443,7 +4488,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7">
       <c r="A120" t="s">
         <v>379</v>
       </c>
@@ -4466,7 +4511,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7">
       <c r="A121" t="s">
         <v>382</v>
       </c>
@@ -4489,7 +4534,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7">
       <c r="A122" t="s">
         <v>385</v>
       </c>
@@ -4512,7 +4557,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7">
       <c r="A123" t="s">
         <v>388</v>
       </c>
@@ -4535,7 +4580,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7">
       <c r="A124" t="s">
         <v>391</v>
       </c>
@@ -4558,7 +4603,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7">
       <c r="A125" t="s">
         <v>394</v>
       </c>
@@ -4581,7 +4626,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7">
       <c r="A126" t="s">
         <v>397</v>
       </c>
@@ -4604,7 +4649,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7">
       <c r="A127" t="s">
         <v>400</v>
       </c>
@@ -4627,7 +4672,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7">
       <c r="A128" t="s">
         <v>403</v>
       </c>
@@ -4650,7 +4695,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7">
       <c r="A129" t="s">
         <v>406</v>
       </c>
@@ -4673,7 +4718,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7">
       <c r="A130" t="s">
         <v>409</v>
       </c>
@@ -4696,7 +4741,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7">
       <c r="A131" t="s">
         <v>412</v>
       </c>
@@ -4721,6 +4766,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4728,22 +4778,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24" style="3" customWidth="1"/>
+    <col min="1" max="1" width="24" style="2" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -4764,19 +4813,22 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="H1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:8" ht="15">
+      <c r="A4" s="3">
         <v>500</v>
       </c>
       <c r="B4" t="s">
@@ -4794,12 +4846,15 @@
       <c r="F4" s="1">
         <v>0.22986111111111099</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="H4" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15">
+      <c r="A5" s="3">
         <v>501</v>
       </c>
       <c r="B5" t="s">
@@ -4817,12 +4872,15 @@
       <c r="F5" s="1">
         <v>0.27152777777777798</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>501</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="H5" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15">
+      <c r="A6" s="3">
         <v>502</v>
       </c>
       <c r="B6" t="s">
@@ -4840,12 +4898,15 @@
       <c r="F6" s="1">
         <v>0.313194444444444</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>502</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="H6" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15">
+      <c r="A7" s="3">
         <v>503</v>
       </c>
       <c r="B7" t="s">
@@ -4863,12 +4924,15 @@
       <c r="F7" s="1">
         <v>0.35486111111111102</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>503</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="H7" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15">
+      <c r="A8" s="3">
         <v>504</v>
       </c>
       <c r="B8" t="s">
@@ -4886,12 +4950,15 @@
       <c r="F8" s="1">
         <v>0.39652777777777798</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>504</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="H8" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15">
+      <c r="A9" s="3">
         <v>505</v>
       </c>
       <c r="B9" t="s">
@@ -4909,12 +4976,15 @@
       <c r="F9" s="1">
         <v>0.438194444444444</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>505</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="H9" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15">
+      <c r="A10" s="3">
         <v>520</v>
       </c>
       <c r="B10" t="s">
@@ -4932,12 +5002,13 @@
       <c r="F10" s="1">
         <v>0.47986111111111113</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>520</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="15">
+      <c r="A11" s="3">
         <v>521</v>
       </c>
       <c r="B11" t="s">
@@ -4955,12 +5026,13 @@
       <c r="F11" s="1">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>521</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" ht="15">
+      <c r="A12" s="3">
         <v>522</v>
       </c>
       <c r="B12" t="s">
@@ -4978,12 +5050,13 @@
       <c r="F12" s="1">
         <v>0.64583333333333337</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>522</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" ht="15">
+      <c r="A13" s="3">
         <v>527</v>
       </c>
       <c r="B13" t="s">
@@ -5001,12 +5074,15 @@
       <c r="F13" s="1">
         <v>0.46875</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>527</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="H13" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15">
+      <c r="A14" s="3">
         <v>537</v>
       </c>
       <c r="B14" t="s">
@@ -5024,12 +5100,15 @@
       <c r="F14" s="1">
         <v>1.1805555555555555E-2</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>537</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="H14" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15">
+      <c r="A15" s="3">
         <v>538</v>
       </c>
       <c r="B15" t="s">
@@ -5047,12 +5126,15 @@
       <c r="F15" s="1">
         <v>9.4444444444444442E-2</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>538</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="H15" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15">
+      <c r="A16" s="3">
         <v>539</v>
       </c>
       <c r="B16" t="s">
@@ -5070,12 +5152,15 @@
       <c r="F16" s="1">
         <v>0.17777777777777778</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>539</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="H16" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15">
+      <c r="A17" s="3">
         <v>540</v>
       </c>
       <c r="B17" t="s">
@@ -5093,12 +5178,15 @@
       <c r="F17" s="1">
         <v>0.26111111111111113</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>540</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="H17" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15">
+      <c r="A18" s="3">
         <v>541</v>
       </c>
       <c r="B18" t="s">
@@ -5116,12 +5204,15 @@
       <c r="F18" s="1">
         <v>0.3444444444444445</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>541</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="H18" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15">
+      <c r="A19" s="3">
         <v>542</v>
       </c>
       <c r="B19" t="s">
@@ -5139,12 +5230,15 @@
       <c r="F19" s="1">
         <v>0.42777777777777781</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>542</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="H19" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15">
+      <c r="A20" s="3">
         <v>547</v>
       </c>
       <c r="B20" t="s">
@@ -5162,12 +5256,13 @@
       <c r="F20" s="1">
         <v>0.51111111111111118</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>547</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" ht="15">
+      <c r="A21" s="3">
         <v>548</v>
       </c>
       <c r="B21" t="s">
@@ -5185,12 +5280,13 @@
       <c r="F21" s="1">
         <v>0.55277777777777781</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>548</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" ht="15">
+      <c r="A22" s="3">
         <v>549</v>
       </c>
       <c r="B22" t="s">
@@ -5208,12 +5304,13 @@
       <c r="F22" s="1">
         <v>0.59444444444444444</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>549</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" ht="15">
+      <c r="A23" s="3">
         <v>550</v>
       </c>
       <c r="B23" t="s">
@@ -5231,12 +5328,15 @@
       <c r="F23" s="1">
         <v>0.63611111111111118</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>550</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="H23" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15">
+      <c r="A24" s="3">
         <v>551</v>
       </c>
       <c r="B24" t="s">
@@ -5254,12 +5354,15 @@
       <c r="F24" s="1">
         <v>0.6777777777777777</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>551</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="H24" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15">
+      <c r="A25" s="3">
         <v>558</v>
       </c>
       <c r="B25" t="s">
@@ -5277,12 +5380,15 @@
       <c r="F25" s="1">
         <v>0.71944444444444444</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <v>558</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="H25" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15">
+      <c r="A26" s="3">
         <v>559</v>
       </c>
       <c r="B26" t="s">
@@ -5300,12 +5406,15 @@
       <c r="F26" s="1">
         <v>0.84375</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <v>559</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="H26" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15">
+      <c r="A27" s="3">
         <v>560</v>
       </c>
       <c r="B27" t="s">
@@ -5323,12 +5432,15 @@
       <c r="F27" s="1">
         <v>0.96875</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>560</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="H27" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15">
+      <c r="A28" s="3">
         <v>561</v>
       </c>
       <c r="B28" t="s">
@@ -5346,12 +5458,15 @@
       <c r="F28" s="1">
         <v>9.375E-2</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <v>561</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="H28" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15">
+      <c r="A29" s="3">
         <v>562</v>
       </c>
       <c r="B29" t="s">
@@ -5369,12 +5484,15 @@
       <c r="F29" s="1">
         <v>0.21875</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>562</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="H29" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15">
+      <c r="A30" s="3">
         <v>563</v>
       </c>
       <c r="B30" t="s">
@@ -5392,12 +5510,15 @@
       <c r="F30" s="1">
         <v>0.34375</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>563</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="H30" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15">
+      <c r="A31" s="3">
         <v>570</v>
       </c>
       <c r="B31" t="s">
@@ -5415,12 +5536,13 @@
       <c r="F31" s="1">
         <v>0.9277777777777777</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <v>570</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" ht="15">
+      <c r="A32" s="3">
         <v>571</v>
       </c>
       <c r="B32" t="s">
@@ -5438,12 +5560,13 @@
       <c r="F32" s="1">
         <v>0.1361111111111111</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <v>571</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" ht="15">
+      <c r="A33" s="3">
         <v>572</v>
       </c>
       <c r="B33" t="s">
@@ -5461,12 +5584,15 @@
       <c r="F33" s="1">
         <v>0.30277777777777776</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <v>572</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="H33" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15">
+      <c r="A34" s="3">
         <v>573</v>
       </c>
       <c r="B34" t="s">
@@ -5484,12 +5610,15 @@
       <c r="F34" s="1">
         <v>0.42777777777777781</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="3">
         <v>573</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="H34" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15">
+      <c r="A35" s="3">
         <v>576</v>
       </c>
       <c r="B35" t="s">
@@ -5507,12 +5636,15 @@
       <c r="F35" s="1">
         <v>0.4861111111111111</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="3">
         <v>576</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="H35" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15">
+      <c r="A36" s="3">
         <v>578</v>
       </c>
       <c r="B36" t="s">
@@ -5530,12 +5662,15 @@
       <c r="F36" s="1">
         <v>0.16666666666666666</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <v>578</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="H36" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15">
+      <c r="A37" s="3">
         <v>579</v>
       </c>
       <c r="B37" t="s">
@@ -5553,12 +5688,15 @@
       <c r="F37" s="1">
         <v>0.25</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="3">
         <v>579</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="H37" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15">
+      <c r="A38" s="3">
         <v>580</v>
       </c>
       <c r="B38" t="s">
@@ -5576,12 +5714,15 @@
       <c r="F38" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="3">
         <v>580</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="H38" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15">
+      <c r="A39" s="3">
         <v>581</v>
       </c>
       <c r="B39" t="s">
@@ -5599,12 +5740,15 @@
       <c r="F39" s="1">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="3">
         <v>581</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="H39" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15">
+      <c r="A40" s="3">
         <v>582</v>
       </c>
       <c r="B40" t="s">
@@ -5622,12 +5766,13 @@
       <c r="F40" s="1">
         <v>0.5</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="3">
         <v>582</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" ht="15">
+      <c r="A41" s="3">
         <v>597</v>
       </c>
       <c r="B41" t="s">
@@ -5645,12 +5790,13 @@
       <c r="F41" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="3">
         <v>597</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" ht="15">
+      <c r="A42" s="3">
         <v>598</v>
       </c>
       <c r="B42" t="s">
@@ -5668,12 +5814,13 @@
       <c r="F42" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="3">
         <v>598</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" ht="15">
+      <c r="A43" s="3">
         <v>599</v>
       </c>
       <c r="B43" t="s">
@@ -5691,12 +5838,15 @@
       <c r="F43" s="1">
         <v>0.625</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="3">
         <v>599</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="H43" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15">
+      <c r="A44" s="3">
         <v>600</v>
       </c>
       <c r="B44" t="s">
@@ -5714,12 +5864,15 @@
       <c r="F44" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="3">
         <v>600</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="H44" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15">
+      <c r="A45" s="3">
         <v>601</v>
       </c>
       <c r="B45" t="s">
@@ -5737,12 +5890,15 @@
       <c r="F45" s="1">
         <v>0.70833333333333337</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45" s="3">
         <v>601</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="H45" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15">
+      <c r="A46" s="3">
         <v>602</v>
       </c>
       <c r="B46" t="s">
@@ -5760,12 +5916,15 @@
       <c r="F46" s="1">
         <v>0.75</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46" s="3">
         <v>602</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="H46" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15">
+      <c r="A47" s="3">
         <v>603</v>
       </c>
       <c r="B47" t="s">
@@ -5783,12 +5942,15 @@
       <c r="F47" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="3">
         <v>603</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="H47" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15">
+      <c r="A48" s="3">
         <v>604</v>
       </c>
       <c r="B48" t="s">
@@ -5806,12 +5968,15 @@
       <c r="F48" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48" s="3">
         <v>604</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+      <c r="H48" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15">
+      <c r="A49" s="3">
         <v>605</v>
       </c>
       <c r="B49" t="s">
@@ -5829,12 +5994,15 @@
       <c r="F49" s="1">
         <v>0.95833333333333337</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49" s="3">
         <v>605</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="H49" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15">
+      <c r="A50" s="3">
         <v>606</v>
       </c>
       <c r="B50" t="s">
@@ -5852,12 +6020,15 @@
       <c r="F50" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="G50" s="4">
+      <c r="G50" s="3">
         <v>606</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="H50" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15">
+      <c r="A51" s="3">
         <v>607</v>
       </c>
       <c r="B51" t="s">
@@ -5875,12 +6046,13 @@
       <c r="F51" s="1">
         <v>0.20833333333333334</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51" s="3">
         <v>607</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="1:8" ht="15">
+      <c r="A52" s="3">
         <v>608</v>
       </c>
       <c r="B52" t="s">
@@ -5898,12 +6070,13 @@
       <c r="F52" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G52" s="4">
+      <c r="G52" s="3">
         <v>608</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="1:8" ht="15">
+      <c r="A53" s="3">
         <v>616</v>
       </c>
       <c r="B53" t="s">
@@ -5921,12 +6094,15 @@
       <c r="F53" s="1">
         <v>0.56041666666666667</v>
       </c>
-      <c r="G53" s="4">
+      <c r="G53" s="3">
         <v>616</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="H53" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15">
+      <c r="A54" s="3">
         <v>622</v>
       </c>
       <c r="B54" t="s">
@@ -5944,12 +6120,15 @@
       <c r="F54" s="1">
         <v>0.23958333333333334</v>
       </c>
-      <c r="G54" s="4">
+      <c r="G54" s="3">
         <v>622</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+      <c r="H54" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15">
+      <c r="A55" s="3">
         <v>623</v>
       </c>
       <c r="B55" t="s">
@@ -5967,12 +6146,15 @@
       <c r="F55" s="1">
         <v>0.32291666666666669</v>
       </c>
-      <c r="G55" s="4">
+      <c r="G55" s="3">
         <v>623</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
+      <c r="H55" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15">
+      <c r="A56" s="3">
         <v>624</v>
       </c>
       <c r="B56" t="s">
@@ -5990,12 +6172,15 @@
       <c r="F56" s="1">
         <v>0.40625</v>
       </c>
-      <c r="G56" s="4">
+      <c r="G56" s="3">
         <v>624</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="H56" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15">
+      <c r="A57" s="3">
         <v>625</v>
       </c>
       <c r="B57" t="s">
@@ -6013,12 +6198,15 @@
       <c r="F57" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="G57" s="4">
+      <c r="G57" s="3">
         <v>625</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+      <c r="H57" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15">
+      <c r="A58" s="3">
         <v>626</v>
       </c>
       <c r="B58" t="s">
@@ -6036,12 +6224,15 @@
       <c r="F58" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="3">
         <v>626</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+      <c r="H58" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15">
+      <c r="A59" s="3">
         <v>627</v>
       </c>
       <c r="B59" t="s">
@@ -6059,12 +6250,15 @@
       <c r="F59" s="1">
         <v>0.57291666666666663</v>
       </c>
-      <c r="G59" s="4">
+      <c r="G59" s="3">
         <v>627</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+      <c r="H59" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15">
+      <c r="A60" s="3">
         <v>628</v>
       </c>
       <c r="B60" t="s">
@@ -6082,12 +6276,15 @@
       <c r="F60" s="1">
         <v>0.61458333333333337</v>
       </c>
-      <c r="G60" s="4">
+      <c r="G60" s="3">
         <v>628</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+      <c r="H60" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15">
+      <c r="A61" s="3">
         <v>633</v>
       </c>
       <c r="B61" t="s">
@@ -6105,12 +6302,15 @@
       <c r="F61" s="1">
         <v>0.73958333333333337</v>
       </c>
-      <c r="G61" s="4">
+      <c r="G61" s="3">
         <v>633</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+      <c r="H61" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15">
+      <c r="A62" s="3">
         <v>634</v>
       </c>
       <c r="B62" t="s">
@@ -6128,12 +6328,15 @@
       <c r="F62" s="1">
         <v>0.78125</v>
       </c>
-      <c r="G62" s="4">
+      <c r="G62" s="3">
         <v>634</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+      <c r="H62" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15">
+      <c r="A63" s="3">
         <v>646</v>
       </c>
       <c r="B63" t="s">
@@ -6151,12 +6354,15 @@
       <c r="F63" s="1">
         <v>0.86458333333333337</v>
       </c>
-      <c r="G63" s="4">
+      <c r="G63" s="3">
         <v>646</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+      <c r="H63" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15">
+      <c r="A64" s="3">
         <v>647</v>
       </c>
       <c r="B64" t="s">
@@ -6174,12 +6380,15 @@
       <c r="F64" s="1">
         <v>0.94791666666666663</v>
       </c>
-      <c r="G64" s="4">
+      <c r="G64" s="3">
         <v>647</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+      <c r="H64" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15">
+      <c r="A65" s="3">
         <v>648</v>
       </c>
       <c r="B65" t="s">
@@ -6197,12 +6406,15 @@
       <c r="F65" s="1">
         <v>7.2916666666666671E-2</v>
       </c>
-      <c r="G65" s="4">
+      <c r="G65" s="3">
         <v>648</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="H65" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15">
+      <c r="A66" s="3">
         <v>649</v>
       </c>
       <c r="B66" t="s">
@@ -6220,12 +6432,15 @@
       <c r="F66" s="1">
         <v>0.19791666666666666</v>
       </c>
-      <c r="G66" s="4">
+      <c r="G66" s="3">
         <v>649</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+      <c r="H66" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15">
+      <c r="A67" s="3">
         <v>650</v>
       </c>
       <c r="B67" t="s">
@@ -6243,12 +6458,15 @@
       <c r="F67" s="1">
         <v>0.50347222222222221</v>
       </c>
-      <c r="G67" s="4">
+      <c r="G67" s="3">
         <v>650</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+      <c r="H67" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15">
+      <c r="A68" s="3">
         <v>654</v>
       </c>
       <c r="B68" t="s">
@@ -6266,12 +6484,15 @@
       <c r="F68" s="1">
         <v>0.88541666666666663</v>
       </c>
-      <c r="G68" s="4">
+      <c r="G68" s="3">
         <v>654</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+      <c r="H68" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15">
+      <c r="A69" s="3">
         <v>655</v>
       </c>
       <c r="B69" t="s">
@@ -6289,12 +6510,13 @@
       <c r="F69" s="1">
         <v>0.96875</v>
       </c>
-      <c r="G69" s="4">
+      <c r="G69" s="3">
         <v>655</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+      <c r="H69" s="3"/>
+    </row>
+    <row r="70" spans="1:8" ht="15">
+      <c r="A70" s="3">
         <v>656</v>
       </c>
       <c r="B70" t="s">
@@ -6312,12 +6534,13 @@
       <c r="F70" s="1">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="G70" s="4">
+      <c r="G70" s="3">
         <v>656</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="1:8" ht="15">
+      <c r="A71" s="3">
         <v>657</v>
       </c>
       <c r="B71" t="s">
@@ -6335,12 +6558,13 @@
       <c r="F71" s="1">
         <v>0.13541666666666666</v>
       </c>
-      <c r="G71" s="4">
+      <c r="G71" s="3">
         <v>657</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="1:8" ht="15">
+      <c r="A72" s="3">
         <v>658</v>
       </c>
       <c r="B72" t="s">
@@ -6358,12 +6582,13 @@
       <c r="F72" s="1">
         <v>0.21875</v>
       </c>
-      <c r="G72" s="4">
+      <c r="G72" s="3">
         <v>658</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="1:8" ht="15">
+      <c r="A73" s="3">
         <v>659</v>
       </c>
       <c r="B73" t="s">
@@ -6381,12 +6606,13 @@
       <c r="F73" s="1">
         <v>0.30208333333333331</v>
       </c>
-      <c r="G73" s="4">
+      <c r="G73" s="3">
         <v>659</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="1:8" ht="15">
+      <c r="A74" s="3">
         <v>660</v>
       </c>
       <c r="B74" t="s">
@@ -6404,12 +6630,15 @@
       <c r="F74" s="1">
         <v>0.34375</v>
       </c>
-      <c r="G74" s="4">
+      <c r="G74" s="3">
         <v>660</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+      <c r="H74" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15">
+      <c r="A75" s="3">
         <v>661</v>
       </c>
       <c r="B75" t="s">
@@ -6427,12 +6656,15 @@
       <c r="F75" s="1">
         <v>0.38541666666666669</v>
       </c>
-      <c r="G75" s="4">
+      <c r="G75" s="3">
         <v>661</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
+      <c r="H75" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15">
+      <c r="A76" s="3">
         <v>662</v>
       </c>
       <c r="B76" t="s">
@@ -6450,12 +6682,15 @@
       <c r="F76" s="1">
         <v>0.42708333333333331</v>
       </c>
-      <c r="G76" s="4">
+      <c r="G76" s="3">
         <v>662</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
+      <c r="H76" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15">
+      <c r="A77" s="3">
         <v>663</v>
       </c>
       <c r="B77" t="s">
@@ -6473,12 +6708,15 @@
       <c r="F77" s="1">
         <v>0.46875</v>
       </c>
-      <c r="G77" s="4">
+      <c r="G77" s="3">
         <v>663</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
+      <c r="H77" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15">
+      <c r="A78" s="3">
         <v>664</v>
       </c>
       <c r="B78" t="s">
@@ -6496,12 +6734,15 @@
       <c r="F78" s="1">
         <v>0.55486111111111114</v>
       </c>
-      <c r="G78" s="4">
+      <c r="G78" s="3">
         <v>664</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="4">
+      <c r="H78" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15">
+      <c r="A79" s="3">
         <v>665</v>
       </c>
       <c r="B79" t="s">
@@ -6519,12 +6760,15 @@
       <c r="F79" s="1">
         <v>0.6381944444444444</v>
       </c>
-      <c r="G79" s="4">
+      <c r="G79" s="3">
         <v>665</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="4">
+      <c r="H79" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15">
+      <c r="A80" s="3">
         <v>666</v>
       </c>
       <c r="B80" t="s">
@@ -6542,12 +6786,15 @@
       <c r="F80" s="1">
         <v>0.72152777777777777</v>
       </c>
-      <c r="G80" s="4">
+      <c r="G80" s="3">
         <v>666</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="4">
+      <c r="H80" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="15">
+      <c r="A81" s="3">
         <v>667</v>
       </c>
       <c r="B81" t="s">
@@ -6565,12 +6812,15 @@
       <c r="F81" s="1">
         <v>0.8881944444444444</v>
       </c>
-      <c r="G81" s="4">
+      <c r="G81" s="3">
         <v>667</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="4">
+      <c r="H81" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15">
+      <c r="A82" s="3">
         <v>669</v>
       </c>
       <c r="B82" t="s">
@@ -6588,12 +6838,13 @@
       <c r="F82" s="1">
         <v>0.22152777777777777</v>
       </c>
-      <c r="G82" s="4">
+      <c r="G82" s="3">
         <v>669</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
+      <c r="H82" s="3"/>
+    </row>
+    <row r="83" spans="1:8" ht="15">
+      <c r="A83" s="3">
         <v>670</v>
       </c>
       <c r="B83" t="s">
@@ -6611,12 +6862,13 @@
       <c r="F83" s="1">
         <v>0.38819444444444445</v>
       </c>
-      <c r="G83" s="4">
+      <c r="G83" s="3">
         <v>670</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="4">
+      <c r="H83" s="3"/>
+    </row>
+    <row r="84" spans="1:8" ht="15">
+      <c r="A84" s="3">
         <v>672</v>
       </c>
       <c r="B84" t="s">
@@ -6634,12 +6886,15 @@
       <c r="F84" s="1">
         <v>0.53472222222222221</v>
       </c>
-      <c r="G84" s="4">
+      <c r="G84" s="3">
         <v>672</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
+      <c r="H84" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15">
+      <c r="A85" s="3">
         <v>679</v>
       </c>
       <c r="B85" t="s">
@@ -6657,12 +6912,15 @@
       <c r="F85" s="1">
         <v>0.4375</v>
       </c>
-      <c r="G85" s="4">
+      <c r="G85" s="3">
         <v>679</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="4">
+      <c r="H85" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15">
+      <c r="A86" s="3">
         <v>680</v>
       </c>
       <c r="B86" t="s">
@@ -6680,12 +6938,15 @@
       <c r="F86" s="1">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G86" s="4">
+      <c r="G86" s="3">
         <v>680</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
+      <c r="H86" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15">
+      <c r="A87" s="3">
         <v>681</v>
       </c>
       <c r="B87" t="s">
@@ -6703,12 +6964,15 @@
       <c r="F87" s="1">
         <v>0.60416666666666663</v>
       </c>
-      <c r="G87" s="4">
+      <c r="G87" s="3">
         <v>681</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
+      <c r="H87" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15">
+      <c r="A88" s="3">
         <v>683</v>
       </c>
       <c r="B88" t="s">
@@ -6726,12 +6990,15 @@
       <c r="F88" s="1">
         <v>0.7284722222222223</v>
       </c>
-      <c r="G88" s="4">
+      <c r="G88" s="3">
         <v>683</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
+      <c r="H88" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15">
+      <c r="A89" s="3">
         <v>684</v>
       </c>
       <c r="B89" t="s">
@@ -6749,12 +7016,15 @@
       <c r="F89" s="1">
         <v>0.81180555555555556</v>
       </c>
-      <c r="G89" s="4">
+      <c r="G89" s="3">
         <v>684</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
+      <c r="H89" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15">
+      <c r="A90" s="3">
         <v>685</v>
       </c>
       <c r="B90" t="s">
@@ -6772,12 +7042,15 @@
       <c r="F90" s="1">
         <v>0.8534722222222223</v>
       </c>
-      <c r="G90" s="4">
+      <c r="G90" s="3">
         <v>685</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
+      <c r="H90" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15">
+      <c r="A91" s="3">
         <v>686</v>
       </c>
       <c r="B91" t="s">
@@ -6795,12 +7068,15 @@
       <c r="F91" s="1">
         <v>0.89513888888888893</v>
       </c>
-      <c r="G91" s="4">
+      <c r="G91" s="3">
         <v>686</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
+      <c r="H91" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15">
+      <c r="A92" s="3">
         <v>687</v>
       </c>
       <c r="B92" t="s">
@@ -6818,12 +7094,15 @@
       <c r="F92" s="1">
         <v>0.93680555555555556</v>
       </c>
-      <c r="G92" s="4">
+      <c r="G92" s="3">
         <v>687</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
+      <c r="H92" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="15">
+      <c r="A93" s="3">
         <v>688</v>
       </c>
       <c r="B93" t="s">
@@ -6841,12 +7120,15 @@
       <c r="F93" s="1">
         <v>0.9784722222222223</v>
       </c>
-      <c r="G93" s="4">
+      <c r="G93" s="3">
         <v>688</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="4">
+      <c r="H93" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="15">
+      <c r="A94" s="3">
         <v>689</v>
       </c>
       <c r="B94" t="s">
@@ -6864,12 +7146,13 @@
       <c r="F94" s="1">
         <v>0.22847222222222222</v>
       </c>
-      <c r="G94" s="4">
+      <c r="G94" s="3">
         <v>689</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
+      <c r="H94" s="3"/>
+    </row>
+    <row r="95" spans="1:8" ht="15">
+      <c r="A95" s="3">
         <v>690</v>
       </c>
       <c r="B95" t="s">
@@ -6887,12 +7170,13 @@
       <c r="F95" s="1">
         <v>0.31180555555555556</v>
       </c>
-      <c r="G95" s="4">
+      <c r="G95" s="3">
         <v>690</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
+      <c r="H95" s="3"/>
+    </row>
+    <row r="96" spans="1:8" ht="15">
+      <c r="A96" s="3">
         <v>691</v>
       </c>
       <c r="B96" t="s">
@@ -6910,12 +7194,13 @@
       <c r="F96" s="1">
         <v>0.39513888888888887</v>
       </c>
-      <c r="G96" s="4">
+      <c r="G96" s="3">
         <v>691</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="4">
+      <c r="H96" s="3"/>
+    </row>
+    <row r="97" spans="1:8" ht="15">
+      <c r="A97" s="3">
         <v>701</v>
       </c>
       <c r="B97" t="s">
@@ -6933,12 +7218,13 @@
       <c r="F97" s="1">
         <v>0.4368055555555555</v>
       </c>
-      <c r="G97" s="4">
+      <c r="G97" s="3">
         <v>701</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
+      <c r="H97" s="3"/>
+    </row>
+    <row r="98" spans="1:8" ht="15">
+      <c r="A98" s="3">
         <v>702</v>
       </c>
       <c r="B98" t="s">
@@ -6956,12 +7242,13 @@
       <c r="F98" s="1">
         <v>0.47847222222222219</v>
       </c>
-      <c r="G98" s="4">
+      <c r="G98" s="3">
         <v>702</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="4">
+      <c r="H98" s="3"/>
+    </row>
+    <row r="99" spans="1:8" ht="15">
+      <c r="A99" s="3">
         <v>703</v>
       </c>
       <c r="B99" t="s">
@@ -6979,12 +7266,13 @@
       <c r="F99" s="1">
         <v>0.52013888888888882</v>
       </c>
-      <c r="G99" s="4">
+      <c r="G99" s="3">
         <v>703</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="4">
+      <c r="H99" s="3"/>
+    </row>
+    <row r="100" spans="1:8" ht="15">
+      <c r="A100" s="3">
         <v>704</v>
       </c>
       <c r="B100" t="s">
@@ -7002,12 +7290,13 @@
       <c r="F100" s="1">
         <v>0.56180555555555556</v>
       </c>
-      <c r="G100" s="4">
+      <c r="G100" s="3">
         <v>704</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="4">
+      <c r="H100" s="3"/>
+    </row>
+    <row r="101" spans="1:8" ht="15">
+      <c r="A101" s="3">
         <v>705</v>
       </c>
       <c r="B101" t="s">
@@ -7025,12 +7314,13 @@
       <c r="F101" s="1">
         <v>0.60347222222222219</v>
       </c>
-      <c r="G101" s="4">
+      <c r="G101" s="3">
         <v>705</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="4">
+      <c r="H101" s="3"/>
+    </row>
+    <row r="102" spans="1:8" ht="15">
+      <c r="A102" s="3">
         <v>706</v>
       </c>
       <c r="B102" t="s">
@@ -7048,12 +7338,13 @@
       <c r="F102" s="1">
         <v>0.64513888888888882</v>
       </c>
-      <c r="G102" s="4">
+      <c r="G102" s="3">
         <v>706</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A103" s="4">
+      <c r="H102" s="3"/>
+    </row>
+    <row r="103" spans="1:8" ht="15">
+      <c r="A103" s="3">
         <v>707</v>
       </c>
       <c r="B103" t="s">
@@ -7071,12 +7362,13 @@
       <c r="F103" s="1">
         <v>0.68680555555555556</v>
       </c>
-      <c r="G103" s="4">
+      <c r="G103" s="3">
         <v>707</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="4">
+      <c r="H103" s="3"/>
+    </row>
+    <row r="104" spans="1:8" ht="15">
+      <c r="A104" s="3">
         <v>708</v>
       </c>
       <c r="B104" t="s">
@@ -7094,12 +7386,13 @@
       <c r="F104" s="1">
         <v>0.7284722222222223</v>
       </c>
-      <c r="G104" s="4">
+      <c r="G104" s="3">
         <v>708</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="4">
+      <c r="H104" s="3"/>
+    </row>
+    <row r="105" spans="1:8" ht="15">
+      <c r="A105" s="3">
         <v>718</v>
       </c>
       <c r="B105" t="s">
@@ -7117,12 +7410,13 @@
       <c r="F105" s="1">
         <v>0.76944444444444438</v>
       </c>
-      <c r="G105" s="4">
+      <c r="G105" s="3">
         <v>718</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="4">
+      <c r="H105" s="3"/>
+    </row>
+    <row r="106" spans="1:8" ht="15">
+      <c r="A106" s="3">
         <v>719</v>
       </c>
       <c r="B106" t="s">
@@ -7140,12 +7434,13 @@
       <c r="F106" s="1">
         <v>0.89444444444444438</v>
       </c>
-      <c r="G106" s="4">
+      <c r="G106" s="3">
         <v>719</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="4">
+      <c r="H106" s="3"/>
+    </row>
+    <row r="107" spans="1:8" ht="15">
+      <c r="A107" s="3">
         <v>720</v>
       </c>
       <c r="B107" t="s">
@@ -7163,12 +7458,13 @@
       <c r="F107" s="1">
         <v>1.9444444444444445E-2</v>
       </c>
-      <c r="G107" s="4">
+      <c r="G107" s="3">
         <v>720</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="4">
+      <c r="H107" s="3"/>
+    </row>
+    <row r="108" spans="1:8" ht="15">
+      <c r="A108" s="3">
         <v>721</v>
       </c>
       <c r="B108" t="s">
@@ -7186,12 +7482,13 @@
       <c r="F108" s="1">
         <v>0.14444444444444446</v>
       </c>
-      <c r="G108" s="4">
+      <c r="G108" s="3">
         <v>721</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="4">
+      <c r="H108" s="3"/>
+    </row>
+    <row r="109" spans="1:8" ht="15">
+      <c r="A109" s="3">
         <v>722</v>
       </c>
       <c r="B109" t="s">
@@ -7209,12 +7506,13 @@
       <c r="F109" s="1">
         <v>0.26944444444444443</v>
       </c>
-      <c r="G109" s="4">
+      <c r="G109" s="3">
         <v>722</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A110" s="4">
+      <c r="H109" s="3"/>
+    </row>
+    <row r="110" spans="1:8" ht="15">
+      <c r="A110" s="3">
         <v>723</v>
       </c>
       <c r="B110" t="s">
@@ -7232,12 +7530,13 @@
       <c r="F110" s="1">
         <v>0.43611111111111112</v>
       </c>
-      <c r="G110" s="4">
+      <c r="G110" s="3">
         <v>723</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="4">
+      <c r="H110" s="3"/>
+    </row>
+    <row r="111" spans="1:8" ht="15">
+      <c r="A111" s="3">
         <v>724</v>
       </c>
       <c r="B111" t="s">
@@ -7255,12 +7554,13 @@
       <c r="F111" s="1">
         <v>0.4777777777777778</v>
       </c>
-      <c r="G111" s="4">
+      <c r="G111" s="3">
         <v>724</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="4">
+      <c r="H111" s="3"/>
+    </row>
+    <row r="112" spans="1:8" ht="15">
+      <c r="A112" s="3">
         <v>738</v>
       </c>
       <c r="B112" t="s">
@@ -7278,12 +7578,13 @@
       <c r="F112" s="1">
         <v>0.64374999999999993</v>
       </c>
-      <c r="G112" s="4">
+      <c r="G112" s="3">
         <v>738</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="4">
+      <c r="H112" s="3"/>
+    </row>
+    <row r="113" spans="1:8" ht="15">
+      <c r="A113" s="3">
         <v>739</v>
       </c>
       <c r="B113" t="s">
@@ -7301,12 +7602,13 @@
       <c r="F113" s="1">
         <v>0.8520833333333333</v>
       </c>
-      <c r="G113" s="4">
+      <c r="G113" s="3">
         <v>739</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="4">
+      <c r="H113" s="3"/>
+    </row>
+    <row r="114" spans="1:8" ht="15">
+      <c r="A114" s="3">
         <v>740</v>
       </c>
       <c r="B114" t="s">
@@ -7324,12 +7626,13 @@
       <c r="F114" s="1">
         <v>6.0416666666666667E-2</v>
       </c>
-      <c r="G114" s="4">
+      <c r="G114" s="3">
         <v>740</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A115" s="4">
+      <c r="H114" s="3"/>
+    </row>
+    <row r="115" spans="1:8" ht="15">
+      <c r="A115" s="3">
         <v>741</v>
       </c>
       <c r="B115" t="s">
@@ -7347,12 +7650,13 @@
       <c r="F115" s="1">
         <v>0.26874999999999999</v>
       </c>
-      <c r="G115" s="4">
+      <c r="G115" s="3">
         <v>741</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="4">
+      <c r="H115" s="3"/>
+    </row>
+    <row r="116" spans="1:8" ht="15">
+      <c r="A116" s="3">
         <v>747</v>
       </c>
       <c r="B116" t="s">
@@ -7370,12 +7674,13 @@
       <c r="F116" s="1">
         <v>0.4513888888888889</v>
       </c>
-      <c r="G116" s="4">
+      <c r="G116" s="3">
         <v>747</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="4">
+      <c r="H116" s="3"/>
+    </row>
+    <row r="117" spans="1:8" ht="15">
+      <c r="A117" s="3">
         <v>795</v>
       </c>
       <c r="B117" t="s">
@@ -7393,12 +7698,13 @@
       <c r="F117" s="1">
         <v>0.39999999999999997</v>
       </c>
-      <c r="G117" s="4">
+      <c r="G117" s="3">
         <v>795</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A118" s="4">
+      <c r="H117" s="3"/>
+    </row>
+    <row r="118" spans="1:8" ht="15">
+      <c r="A118" s="3">
         <v>833</v>
       </c>
       <c r="B118" t="s">
@@ -7416,12 +7722,13 @@
       <c r="F118" s="1">
         <v>0.51874999999999993</v>
       </c>
-      <c r="G118" s="4">
+      <c r="G118" s="3">
         <v>833</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A119" s="4">
+      <c r="H118" s="3"/>
+    </row>
+    <row r="119" spans="1:8" ht="15">
+      <c r="A119" s="3">
         <v>867</v>
       </c>
       <c r="B119" t="s">
@@ -7439,12 +7746,13 @@
       <c r="F119" s="1">
         <v>0.53680555555555554</v>
       </c>
-      <c r="G119" s="4">
+      <c r="G119" s="3">
         <v>867</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="4">
+      <c r="H119" s="3"/>
+    </row>
+    <row r="120" spans="1:8" ht="15">
+      <c r="A120" s="3">
         <v>880</v>
       </c>
       <c r="B120" t="s">
@@ -7462,12 +7770,13 @@
       <c r="F120" s="1">
         <v>0.78125</v>
       </c>
-      <c r="G120" s="4">
+      <c r="G120" s="3">
         <v>880</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A121" s="4">
+      <c r="H120" s="3"/>
+    </row>
+    <row r="121" spans="1:8" ht="15">
+      <c r="A121" s="3">
         <v>881</v>
       </c>
       <c r="B121" t="s">
@@ -7485,12 +7794,13 @@
       <c r="F121" s="1">
         <v>0.86458333333333337</v>
       </c>
-      <c r="G121" s="4">
+      <c r="G121" s="3">
         <v>881</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A122" s="4">
+      <c r="H121" s="3"/>
+    </row>
+    <row r="122" spans="1:8" ht="15">
+      <c r="A122" s="3">
         <v>882</v>
       </c>
       <c r="B122" t="s">
@@ -7508,12 +7818,13 @@
       <c r="F122" s="1">
         <v>0.94791666666666663</v>
       </c>
-      <c r="G122" s="4">
+      <c r="G122" s="3">
         <v>882</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A123" s="4">
+      <c r="H122" s="3"/>
+    </row>
+    <row r="123" spans="1:8" ht="15">
+      <c r="A123" s="3">
         <v>883</v>
       </c>
       <c r="B123" t="s">
@@ -7531,12 +7842,13 @@
       <c r="F123" s="1">
         <v>3.125E-2</v>
       </c>
-      <c r="G123" s="4">
+      <c r="G123" s="3">
         <v>883</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A124" s="4">
+      <c r="H123" s="3"/>
+    </row>
+    <row r="124" spans="1:8" ht="15">
+      <c r="A124" s="3">
         <v>884</v>
       </c>
       <c r="B124" t="s">
@@ -7554,12 +7866,13 @@
       <c r="F124" s="1">
         <v>0.11458333333333333</v>
       </c>
-      <c r="G124" s="4">
+      <c r="G124" s="3">
         <v>884</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A125" s="4">
+      <c r="H124" s="3"/>
+    </row>
+    <row r="125" spans="1:8" ht="15">
+      <c r="A125" s="3">
         <v>885</v>
       </c>
       <c r="B125" t="s">
@@ -7577,12 +7890,13 @@
       <c r="F125" s="1">
         <v>0.19791666666666666</v>
       </c>
-      <c r="G125" s="4">
+      <c r="G125" s="3">
         <v>885</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A126" s="4">
+      <c r="H125" s="3"/>
+    </row>
+    <row r="126" spans="1:8" ht="15">
+      <c r="A126" s="3">
         <v>886</v>
       </c>
       <c r="B126" t="s">
@@ -7600,12 +7914,13 @@
       <c r="F126" s="1">
         <v>0.28125</v>
       </c>
-      <c r="G126" s="4">
+      <c r="G126" s="3">
         <v>886</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A127" s="4">
+      <c r="H126" s="3"/>
+    </row>
+    <row r="127" spans="1:8" ht="15">
+      <c r="A127" s="3">
         <v>887</v>
       </c>
       <c r="B127" t="s">
@@ -7623,12 +7938,13 @@
       <c r="F127" s="1">
         <v>0.36458333333333331</v>
       </c>
-      <c r="G127" s="4">
+      <c r="G127" s="3">
         <v>887</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A128" s="4">
+      <c r="H127" s="3"/>
+    </row>
+    <row r="128" spans="1:8" ht="15">
+      <c r="A128" s="3">
         <v>888</v>
       </c>
       <c r="B128" t="s">
@@ -7646,12 +7962,13 @@
       <c r="F128" s="1">
         <v>0.44791666666666669</v>
       </c>
-      <c r="G128" s="4">
+      <c r="G128" s="3">
         <v>888</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A129" s="4">
+      <c r="H128" s="3"/>
+    </row>
+    <row r="129" spans="1:8" ht="15">
+      <c r="A129" s="3">
         <v>889</v>
       </c>
       <c r="B129" t="s">
@@ -7669,12 +7986,13 @@
       <c r="F129" s="1">
         <v>0.53125</v>
       </c>
-      <c r="G129" s="4">
+      <c r="G129" s="3">
         <v>889</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A130" s="4">
+      <c r="H129" s="3"/>
+    </row>
+    <row r="130" spans="1:8" ht="15">
+      <c r="A130" s="3">
         <v>894</v>
       </c>
       <c r="B130" t="s">
@@ -7692,12 +8010,13 @@
       <c r="F130" s="1">
         <v>0.65069444444444446</v>
       </c>
-      <c r="G130" s="4">
+      <c r="G130" s="3">
         <v>894</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A131" s="4">
+      <c r="H130" s="3"/>
+    </row>
+    <row r="131" spans="1:8" ht="15">
+      <c r="A131" s="3">
         <v>895</v>
       </c>
       <c r="B131" t="s">
@@ -7715,12 +8034,13 @@
       <c r="F131" s="1">
         <v>0.81736111111111109</v>
       </c>
-      <c r="G131" s="4">
+      <c r="G131" s="3">
         <v>895</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A132" s="4">
+      <c r="H131" s="3"/>
+    </row>
+    <row r="132" spans="1:8" ht="15">
+      <c r="A132" s="3">
         <v>896</v>
       </c>
       <c r="B132" t="s">
@@ -7738,12 +8058,13 @@
       <c r="F132" s="1">
         <v>2.5694444444444447E-2</v>
       </c>
-      <c r="G132" s="4">
+      <c r="G132" s="3">
         <v>896</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="4">
+      <c r="H132" s="3"/>
+    </row>
+    <row r="133" spans="1:8" ht="15">
+      <c r="A133" s="3">
         <v>897</v>
       </c>
       <c r="B133" t="s">
@@ -7761,12 +8082,13 @@
       <c r="F133" s="1">
         <v>0.19236111111111112</v>
       </c>
-      <c r="G133" s="4">
+      <c r="G133" s="3">
         <v>897</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A134" s="4">
+      <c r="H133" s="3"/>
+    </row>
+    <row r="134" spans="1:8" ht="15">
+      <c r="A134" s="3">
         <v>898</v>
       </c>
       <c r="B134" t="s">
@@ -7784,12 +8106,13 @@
       <c r="F134" s="1">
         <v>0.35902777777777778</v>
       </c>
-      <c r="G134" s="4">
+      <c r="G134" s="3">
         <v>898</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A135" s="4">
+      <c r="H134" s="3"/>
+    </row>
+    <row r="135" spans="1:8" ht="15">
+      <c r="A135" s="3">
         <v>902</v>
       </c>
       <c r="B135" t="s">
@@ -7807,12 +8130,13 @@
       <c r="F135" s="1">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G135" s="4">
+      <c r="G135" s="3">
         <v>902</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A136" s="4">
+      <c r="H135" s="3"/>
+    </row>
+    <row r="136" spans="1:8" ht="15">
+      <c r="A136" s="3">
         <v>903</v>
       </c>
       <c r="B136" t="s">
@@ -7830,12 +8154,13 @@
       <c r="F136" s="1">
         <v>0.10416666666666667</v>
       </c>
-      <c r="G136" s="4">
+      <c r="G136" s="3">
         <v>903</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A137" s="4">
+      <c r="H136" s="3"/>
+    </row>
+    <row r="137" spans="1:8" ht="15">
+      <c r="A137" s="3">
         <v>904</v>
       </c>
       <c r="B137" t="s">
@@ -7853,12 +8178,13 @@
       <c r="F137" s="1">
         <v>0.1875</v>
       </c>
-      <c r="G137" s="4">
+      <c r="G137" s="3">
         <v>904</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A138" s="4">
+      <c r="H137" s="3"/>
+    </row>
+    <row r="138" spans="1:8" ht="15">
+      <c r="A138" s="3">
         <v>905</v>
       </c>
       <c r="B138" t="s">
@@ -7876,12 +8202,13 @@
       <c r="F138" s="1">
         <v>0.22916666666666666</v>
       </c>
-      <c r="G138" s="4">
+      <c r="G138" s="3">
         <v>905</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A139" s="4">
+      <c r="H138" s="3"/>
+    </row>
+    <row r="139" spans="1:8" ht="15">
+      <c r="A139" s="3">
         <v>906</v>
       </c>
       <c r="B139" t="s">
@@ -7899,12 +8226,13 @@
       <c r="F139" s="1">
         <v>0.27083333333333331</v>
       </c>
-      <c r="G139" s="4">
+      <c r="G139" s="3">
         <v>906</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A140" s="4">
+      <c r="H139" s="3"/>
+    </row>
+    <row r="140" spans="1:8" ht="15">
+      <c r="A140" s="3">
         <v>907</v>
       </c>
       <c r="B140" t="s">
@@ -7922,12 +8250,13 @@
       <c r="F140" s="1">
         <v>0.31388888888888888</v>
       </c>
-      <c r="G140" s="4">
+      <c r="G140" s="3">
         <v>907</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A141" s="4">
+      <c r="H140" s="3"/>
+    </row>
+    <row r="141" spans="1:8" ht="15">
+      <c r="A141" s="3">
         <v>908</v>
       </c>
       <c r="B141" t="s">
@@ -7945,12 +8274,13 @@
       <c r="F141" s="1">
         <v>0.39583333333333331</v>
       </c>
-      <c r="G141" s="4">
+      <c r="G141" s="3">
         <v>908</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A142" s="4">
+      <c r="H141" s="3"/>
+    </row>
+    <row r="142" spans="1:8" ht="15">
+      <c r="A142" s="3">
         <v>913</v>
       </c>
       <c r="B142" t="s">
@@ -7968,12 +8298,13 @@
       <c r="F142" s="1">
         <v>0.6020833333333333</v>
       </c>
-      <c r="G142" s="4">
+      <c r="G142" s="3">
         <v>913</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A143" s="4">
+      <c r="H142" s="3"/>
+    </row>
+    <row r="143" spans="1:8" ht="15">
+      <c r="A143" s="3">
         <v>914</v>
       </c>
       <c r="B143" t="s">
@@ -7991,12 +8322,13 @@
       <c r="F143" s="1">
         <v>0.93541666666666667</v>
       </c>
-      <c r="G143" s="4">
+      <c r="G143" s="3">
         <v>914</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A144" s="4">
+      <c r="H143" s="3"/>
+    </row>
+    <row r="144" spans="1:8" ht="15">
+      <c r="A144" s="3">
         <v>915</v>
       </c>
       <c r="B144" t="s">
@@ -8014,12 +8346,15 @@
       <c r="F144" s="1">
         <v>0.43541666666666662</v>
       </c>
-      <c r="G144" s="4">
+      <c r="G144" s="3">
         <v>915</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A145" s="4">
+      <c r="H144" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="15">
+      <c r="A145" s="3">
         <v>916</v>
       </c>
       <c r="B145" t="s">
@@ -8037,12 +8372,15 @@
       <c r="F145" s="1">
         <v>0.59722222222222221</v>
       </c>
-      <c r="G145" s="4">
+      <c r="G145" s="3">
         <v>916</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A146" s="4">
+      <c r="H145" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="15">
+      <c r="A146" s="3">
         <v>917</v>
       </c>
       <c r="B146" t="s">
@@ -8060,12 +8398,15 @@
       <c r="F146" s="1">
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="G146" s="4">
+      <c r="G146" s="3">
         <v>917</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A147" s="4">
+      <c r="H146" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="15">
+      <c r="A147" s="3">
         <v>921</v>
       </c>
       <c r="B147" t="s">
@@ -8083,12 +8424,20 @@
       <c r="F147" s="1">
         <v>0.51041666666666663</v>
       </c>
-      <c r="G147" s="4">
+      <c r="G147" s="3">
         <v>921</v>
+      </c>
+      <c r="H147" s="3" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>